<commit_message>
verification of strat matrix
</commit_message>
<xml_diff>
--- a/III.2- Strategy/Strategy Matrix/matrix good version.xlsx
+++ b/III.2- Strategy/Strategy Matrix/matrix good version.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Human Resource</t>
   </si>
@@ -190,6 +190,9 @@
   <si>
     <t>Support academic to do more  research about EV charging efficiency and effectiveness</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,8 +233,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -425,22 +434,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -459,6 +474,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -495,8 +513,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,7 +592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,7 +627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -804,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,31 +860,31 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="22" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
@@ -861,176 +895,181 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="6" t="s">
+    <row r="8" spans="1:5" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="44" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="34" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="17" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="28" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="21" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="21"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="28" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="22" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="23"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1039,22 +1078,23 @@
       <c r="D19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="27"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B19:B20"/>

</xml_diff>